<commit_message>
sample pdf and import success message redirection issue solved
sample pdf and import success message redirection issue solved
</commit_message>
<xml_diff>
--- a/path_to_your_upload_directory/Book2.xlsx
+++ b/path_to_your_upload_directory/Book2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="6030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>name</t>
   </si>
@@ -38,52 +38,19 @@
     <t>categoryid</t>
   </si>
   <si>
-    <t>cuisineid</t>
-  </si>
-  <si>
-    <t>indhu</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>chappathi</t>
-  </si>
-  <si>
-    <t>biriyani</t>
-  </si>
-  <si>
-    <t>xc</t>
-  </si>
-  <si>
-    <t>dosa</t>
-  </si>
-  <si>
-    <t>zxc</t>
-  </si>
-  <si>
-    <t>itli</t>
-  </si>
-  <si>
-    <t>mango</t>
-  </si>
-  <si>
-    <t>orange</t>
-  </si>
-  <si>
-    <t>biscuit</t>
-  </si>
-  <si>
-    <t>dfs</t>
-  </si>
-  <si>
-    <t>Tomato</t>
-  </si>
-  <si>
-    <t>thosa</t>
-  </si>
-  <si>
-    <t>piece</t>
+    <t>onion</t>
+  </si>
+  <si>
+    <t>ltr</t>
+  </si>
+  <si>
+    <t>powder</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>juice</t>
   </si>
 </sst>
 </file>
@@ -408,15 +375,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,228 +396,46 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2">
-        <v>5</v>
+        <v>5554</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
       <c r="C3">
-        <v>5</v>
+        <v>455</v>
       </c>
       <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9">
-        <v>6</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10">
-        <v>6</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11">
-        <v>6</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12">
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
-        <v>6</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14">
-        <v>30</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
         <v>1</v>
       </c>
     </row>

</xml_diff>